<commit_message>
Added the logic of Hashtable in Dataprovider
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agupta/eclipse-workspace/APITestingFramework/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A65438A-9235-854A-8FB4-CCADEE8F1D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65515453-8020-D646-8C0A-6E3C79F1090A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" activeTab="2" xr2:uid="{D90C72EB-1969-FB4D-A4FF-9D961660326E}"/>
   </bookViews>
@@ -76,12 +76,6 @@
     <t>Adding the third customer</t>
   </si>
   <si>
-    <t>validCreateCustomerAPI</t>
-  </si>
-  <si>
-    <t>invalidCreateCustomerAPI</t>
-  </si>
-  <si>
     <t>deleteCustomerAPI</t>
   </si>
   <si>
@@ -92,6 +86,12 @@
   </si>
   <si>
     <t>cus_PcwoVgUG5zFe05</t>
+  </si>
+  <si>
+    <t>test01_ValidCreateCustomerAPI</t>
+  </si>
+  <si>
+    <t>test02_InvalidCreateCustomerAPI</t>
   </si>
 </sst>
 </file>
@@ -583,18 +583,18 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -643,7 +643,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -681,22 +681,22 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>